<commit_message>
FIFO: change ram type & output pattern
</commit_message>
<xml_diff>
--- a/lab2_resource/control.xlsx
+++ b/lab2_resource/control.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>State</t>
   </si>
@@ -33,9 +33,6 @@
     <t>ctr_en</t>
   </si>
   <si>
-    <t>ram_en</t>
-  </si>
-  <si>
     <t>ram_we</t>
   </si>
   <si>
@@ -57,7 +54,7 @@
     <t>x</t>
   </si>
   <si>
-    <t>HOLD</t>
+    <t>outr_en</t>
   </si>
 </sst>
 </file>
@@ -375,15 +372,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection sqref="A1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="9.06640625" customWidth="1"/>
+    <col min="3" max="3" width="9.06640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
@@ -394,27 +391,27 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -432,30 +429,30 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -466,19 +463,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -488,32 +485,6 @@
       </c>
       <c r="H4">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>